<commit_message>
static analysis & doxygen done
</commit_message>
<xml_diff>
--- a/documents/Novec1230_container_discharge.xlsx
+++ b/documents/Novec1230_container_discharge.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>Percent Outage</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>Henry's Const = 3600</t>
+  </si>
+  <si>
+    <t>Container Pressure (PSI)</t>
+  </si>
+  <si>
+    <t>VB code from Tom</t>
   </si>
 </sst>
 </file>
@@ -77,8 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,11 +457,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="256893608"/>
-        <c:axId val="256894000"/>
+        <c:axId val="263607176"/>
+        <c:axId val="263607568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="256893608"/>
+        <c:axId val="263607176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -571,12 +580,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256894000"/>
+        <c:crossAx val="263607568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="256894000"/>
+        <c:axId val="263607568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -702,7 +711,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256893608"/>
+        <c:crossAx val="263607176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -806,7 +815,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1328,11 +1337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="280536128"/>
-        <c:axId val="280531032"/>
+        <c:axId val="263608352"/>
+        <c:axId val="263608744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="280536128"/>
+        <c:axId val="263608352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1352,6 +1361,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Percent Outage</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1389,12 +1459,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280531032"/>
+        <c:crossAx val="263608744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="280531032"/>
+        <c:axId val="263608744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,6 +1484,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Container Pressure (psig)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1451,7 +1582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="280536128"/>
+        <c:crossAx val="263608352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1463,6 +1594,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2647,15 +2810,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>838199</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3611,8 +3774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3624,21 +3787,29 @@
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -3659,6 +3830,15 @@
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="I2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -4573,10 +4753,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="I1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Novec property file with Henry's const
</commit_message>
<xml_diff>
--- a/documents/Novec1230_container_discharge.xlsx
+++ b/documents/Novec1230_container_discharge.xlsx
@@ -457,11 +457,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="563757520"/>
-        <c:axId val="563757912"/>
+        <c:axId val="308195336"/>
+        <c:axId val="308195728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="563757520"/>
+        <c:axId val="308195336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -580,12 +580,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="563757912"/>
+        <c:crossAx val="308195728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="563757912"/>
+        <c:axId val="308195728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -711,7 +711,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="563757520"/>
+        <c:crossAx val="308195336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1337,11 +1337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="563758696"/>
-        <c:axId val="563759088"/>
+        <c:axId val="308196512"/>
+        <c:axId val="308196904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="563758696"/>
+        <c:axId val="308196512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,12 +1459,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="563759088"/>
+        <c:crossAx val="308196904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="563759088"/>
+        <c:axId val="308196904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,7 +1582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="563758696"/>
+        <c:crossAx val="308196512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3930,7 +3930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>

</xml_diff>